<commit_message>
Adicionando telas ao programa
Adicionando o botão de "Menu" ao programa. Adicionando mais telas ao programa.
</commit_message>
<xml_diff>
--- a/ListaPecas.xlsx
+++ b/ListaPecas.xlsx
@@ -468,10 +468,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -482,6 +482,7 @@
     <col width="18.7109375" customWidth="1" min="4" max="4"/>
     <col width="27.5703125" customWidth="1" min="5" max="5"/>
     <col width="26.5703125" customWidth="1" style="7" min="6" max="6"/>
+    <col width="10.85546875" customWidth="1" style="7" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -515,6 +516,11 @@
           <t>Caixa</t>
         </is>
       </c>
+      <c r="G1" s="7" t="inlineStr">
+        <is>
+          <t>Somatorio</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
@@ -545,6 +551,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G2" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="inlineStr">
@@ -575,6 +586,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="inlineStr">
@@ -605,6 +621,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="inlineStr">
@@ -635,6 +656,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="inlineStr">
@@ -665,6 +691,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="inlineStr">
@@ -695,6 +726,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="inlineStr">
@@ -725,6 +761,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="inlineStr">
@@ -755,6 +796,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="inlineStr">
@@ -785,6 +831,11 @@
           <t xml:space="preserve">G2 e G3 </t>
         </is>
       </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="inlineStr">
@@ -815,6 +866,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
@@ -845,6 +901,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="inlineStr">
@@ -875,6 +936,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G13" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="inlineStr">
@@ -905,6 +971,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G14" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="inlineStr">
@@ -935,6 +1006,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="inlineStr">
@@ -965,6 +1041,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G16" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="inlineStr">
@@ -995,6 +1076,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G17" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="inlineStr">
@@ -1025,6 +1111,11 @@
           <t>G6 Play/H1</t>
         </is>
       </c>
+      <c r="G18" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="inlineStr">
@@ -1055,6 +1146,11 @@
           <t>G6 Play</t>
         </is>
       </c>
+      <c r="G19" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="inlineStr">
@@ -1085,6 +1181,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G20" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="inlineStr">
@@ -1115,6 +1216,11 @@
           <t>Motorola Caixa 1</t>
         </is>
       </c>
+      <c r="G21" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="inlineStr">
@@ -1142,7 +1248,12 @@
       </c>
       <c r="F22" s="7" t="inlineStr">
         <is>
-          <t>G7 Play/H1</t>
+          <t>G7 Play</t>
+        </is>
+      </c>
+      <c r="G22" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1168,11 +1279,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 2/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G23" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1194,15 +1310,20 @@
       </c>
       <c r="D24" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F24" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G24" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1212,14 +1333,14 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
-        <is>
-          <t>Moto G7/Moto G7 Plus</t>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>Moto E7</t>
         </is>
       </c>
       <c r="C25" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D25" s="7" t="inlineStr">
@@ -1228,11 +1349,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>E24</t>
         </is>
       </c>
     </row>
@@ -1242,14 +1368,14 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>Moto G8 Play</t>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>Moto E7 Power</t>
         </is>
       </c>
       <c r="C26" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D26" s="7" t="inlineStr">
@@ -1262,7 +1388,12 @@
       </c>
       <c r="F26" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 2/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>E24</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1405,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Moto G8 Plus</t>
+          <t>Moto G7/Moto G7 Plus</t>
         </is>
       </c>
       <c r="C27" s="7" t="inlineStr">
@@ -1293,6 +1424,11 @@
       <c r="F27" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1304,7 +1440,7 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>Moto G8 Power</t>
+          <t>Moto G8 Play</t>
         </is>
       </c>
       <c r="C28" s="7" t="inlineStr">
@@ -1322,7 +1458,12 @@
       </c>
       <c r="F28" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 2/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G28" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1475,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>Moto G8 Power Lite</t>
+          <t>Moto G8 Plus</t>
         </is>
       </c>
       <c r="C29" s="7" t="inlineStr">
@@ -1348,11 +1489,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 2/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1510,7 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>Moto G8</t>
+          <t>Moto G8 Power</t>
         </is>
       </c>
       <c r="C30" s="7" t="inlineStr">
@@ -1378,11 +1524,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 2/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1545,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>Moto G9 Play/ Moto E7 Plus</t>
+          <t>Moto G8 Power Lite</t>
         </is>
       </c>
       <c r="C31" s="7" t="inlineStr">
@@ -1404,15 +1555,20 @@
       </c>
       <c r="D31" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4</t>
+          <t>Motorola Caixa 2/H1</t>
+        </is>
+      </c>
+      <c r="G31" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1422,9 +1578,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B32" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Moto G9 Play </t>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>Moto G8</t>
         </is>
       </c>
       <c r="C32" s="7" t="inlineStr">
@@ -1442,7 +1598,12 @@
       </c>
       <c r="F32" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4/ H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G32" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1452,9 +1613,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B33" s="6" t="inlineStr">
-        <is>
-          <t>Moto G9 Plus</t>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>Moto G9 Play/ Moto E7 Plus</t>
         </is>
       </c>
       <c r="C33" s="7" t="inlineStr">
@@ -1464,15 +1625,20 @@
       </c>
       <c r="D33" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4</t>
+          <t>Motorola Caixa 4/H1</t>
+        </is>
+      </c>
+      <c r="G33" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1482,9 +1648,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>Moto G10</t>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>Moto G9 Plus</t>
         </is>
       </c>
       <c r="C34" s="7" t="inlineStr">
@@ -1494,15 +1660,20 @@
       </c>
       <c r="D34" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G34" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1512,9 +1683,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B35" s="3" t="inlineStr">
-        <is>
-          <t>Moto G20</t>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>Moto G10/G20/G30</t>
         </is>
       </c>
       <c r="C35" s="7" t="inlineStr">
@@ -1528,11 +1699,16 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4</t>
+          <t>Motorola Caixa 4/H1</t>
+        </is>
+      </c>
+      <c r="G35" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1542,9 +1718,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B36" s="2" t="inlineStr">
-        <is>
-          <t>Moto G30</t>
+      <c r="B36" s="6" t="inlineStr">
+        <is>
+          <t>Moto E20</t>
         </is>
       </c>
       <c r="C36" s="7" t="inlineStr">
@@ -1554,15 +1730,20 @@
       </c>
       <c r="D36" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4/H1</t>
+          <t>Motorola Caixa 2</t>
+        </is>
+      </c>
+      <c r="G36" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1584,15 +1765,20 @@
       </c>
       <c r="D37" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G37" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1602,9 +1788,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B38" s="2" t="inlineStr">
-        <is>
-          <t>Moto One</t>
+      <c r="B38" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Moto One Action </t>
         </is>
       </c>
       <c r="C38" s="7" t="inlineStr">
@@ -1618,11 +1804,16 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G38" s="7" t="inlineStr">
+        <is>
+          <t>E37</t>
         </is>
       </c>
     </row>
@@ -1632,9 +1823,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B39" s="3" t="inlineStr">
-        <is>
-          <t>Moto One Fusion Plus</t>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Moto One Vision</t>
         </is>
       </c>
       <c r="C39" s="7" t="inlineStr">
@@ -1648,11 +1839,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G39" s="7" t="inlineStr">
+        <is>
+          <t>E37</t>
         </is>
       </c>
     </row>
@@ -1664,7 +1860,7 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>Moto E4 Plus C/Aro Azul</t>
+          <t>Moto One</t>
         </is>
       </c>
       <c r="C40" s="7" t="inlineStr">
@@ -1674,7 +1870,7 @@
       </c>
       <c r="D40" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -1682,7 +1878,12 @@
       </c>
       <c r="F40" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 1</t>
+          <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G40" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1694,7 +1895,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Moto E5 Play</t>
+          <t>Moto One Fusion Plus</t>
         </is>
       </c>
       <c r="C41" s="7" t="inlineStr">
@@ -1704,15 +1905,20 @@
       </c>
       <c r="D41" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 1</t>
+          <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G41" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1724,7 +1930,7 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>Moto E6S/ E6i</t>
+          <t>Moto E4 Plus C/Aro Azul</t>
         </is>
       </c>
       <c r="C42" s="7" t="inlineStr">
@@ -1734,15 +1940,20 @@
       </c>
       <c r="D42" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Médio Baixo</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4</t>
+          <t>Motorola Caixa 1</t>
+        </is>
+      </c>
+      <c r="G42" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1754,7 +1965,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>Moto E6 Play</t>
+          <t>Moto E5 Play</t>
         </is>
       </c>
       <c r="C43" s="7" t="inlineStr">
@@ -1764,15 +1975,20 @@
       </c>
       <c r="D43" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 4</t>
+          <t>Motorola Caixa 1</t>
+        </is>
+      </c>
+      <c r="G43" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1782,9 +1998,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B44" s="6" t="inlineStr">
-        <is>
-          <t>Moto E7 Plus</t>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>Moto E6S/ E6i</t>
         </is>
       </c>
       <c r="C44" s="7" t="inlineStr">
@@ -1794,7 +2010,7 @@
       </c>
       <c r="D44" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t xml:space="preserve"> Médio Baixo</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -1805,6 +2021,11 @@
           <t>Motorola Caixa 4</t>
         </is>
       </c>
+      <c r="G44" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="inlineStr">
@@ -1812,9 +2033,9 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B45" s="2" t="inlineStr">
-        <is>
-          <t>Moto X4</t>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>Moto E6 Play</t>
         </is>
       </c>
       <c r="C45" s="7" t="inlineStr">
@@ -1824,15 +2045,20 @@
       </c>
       <c r="D45" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="7" t="inlineStr">
         <is>
-          <t>Motorola Caixa 1</t>
+          <t>Motorola Caixa 4</t>
+        </is>
+      </c>
+      <c r="G45" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1842,57 +2068,67 @@
           <t>Motorola</t>
         </is>
       </c>
-      <c r="B46" s="3" t="inlineStr">
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>Moto X4</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>Preta</t>
+        </is>
+      </c>
+      <c r="D46" s="7" t="inlineStr">
+        <is>
+          <t>Exceção</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7" t="inlineStr">
+        <is>
+          <t>Motorola Caixa 1</t>
+        </is>
+      </c>
+      <c r="G46" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Motorola</t>
+        </is>
+      </c>
+      <c r="B47" s="3" t="inlineStr">
         <is>
           <t>Moto C Plus</t>
         </is>
       </c>
-      <c r="C46" s="7" t="inlineStr">
+      <c r="C47" s="7" t="inlineStr">
         <is>
           <t>Dourada</t>
         </is>
       </c>
-      <c r="D46" s="7" t="inlineStr">
+      <c r="D47" s="7" t="inlineStr">
         <is>
           <t>Exceção</t>
         </is>
       </c>
-      <c r="E46" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7" t="inlineStr">
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7" t="inlineStr">
         <is>
           <t>Motorola Caixa 1</t>
         </is>
       </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="7" t="inlineStr">
-        <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-      <c r="B47" s="2" t="inlineStr">
-        <is>
-          <t>J2 Core</t>
-        </is>
-      </c>
-      <c r="C47" s="7" t="inlineStr">
-        <is>
-          <t>Preta</t>
-        </is>
-      </c>
-      <c r="D47" s="7" t="inlineStr">
-        <is>
-          <t>Médio</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7" t="inlineStr">
-        <is>
-          <t>Samsung Orig. Importada</t>
+      <c r="G47" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1902,19 +2138,19 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B48" s="3" t="inlineStr">
-        <is>
-          <t>J4</t>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>J2 Core</t>
         </is>
       </c>
       <c r="C48" s="7" t="inlineStr">
         <is>
-          <t>Azul</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D48" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1923,6 +2159,11 @@
       <c r="F48" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G48" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1932,27 +2173,32 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B49" s="2" t="inlineStr">
+      <c r="B49" s="3" t="inlineStr">
         <is>
           <t>J4</t>
         </is>
       </c>
       <c r="C49" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Azul</t>
         </is>
       </c>
       <c r="D49" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G49" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1962,9 +2208,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B50" s="3" t="inlineStr">
-        <is>
-          <t>J5</t>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>J4</t>
         </is>
       </c>
       <c r="C50" s="7" t="inlineStr">
@@ -1974,15 +2220,20 @@
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G50" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -1992,27 +2243,32 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B51" s="2" t="inlineStr">
-        <is>
-          <t>J5 Prime</t>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>J5</t>
         </is>
       </c>
       <c r="C51" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D51" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F51" s="7" t="inlineStr">
         <is>
-          <t>J5 Prime</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G51" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2022,14 +2278,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B52" s="3" t="inlineStr">
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>J5 Prime</t>
         </is>
       </c>
       <c r="C52" s="7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D52" s="7" t="inlineStr">
@@ -2038,11 +2294,16 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F52" s="7" t="inlineStr">
         <is>
           <t>J5 Prime</t>
+        </is>
+      </c>
+      <c r="G52" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2052,14 +2313,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B53" s="2" t="inlineStr">
-        <is>
-          <t>J5 Pro</t>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>J5 Prime</t>
         </is>
       </c>
       <c r="C53" s="7" t="inlineStr">
         <is>
-          <t>Dourada</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="D53" s="7" t="inlineStr">
@@ -2068,11 +2329,16 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="7" t="inlineStr">
         <is>
-          <t>Samsung Orig. Importada</t>
+          <t>J5 Prime</t>
+        </is>
+      </c>
+      <c r="G53" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2082,14 +2348,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B54" s="3" t="inlineStr">
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>J5 Pro</t>
         </is>
       </c>
       <c r="C54" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Dourada</t>
         </is>
       </c>
       <c r="D54" s="7" t="inlineStr">
@@ -2103,6 +2369,11 @@
       <c r="F54" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G54" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2112,9 +2383,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B55" s="2" t="inlineStr">
-        <is>
-          <t>J6</t>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>J5 Pro</t>
         </is>
       </c>
       <c r="C55" s="7" t="inlineStr">
@@ -2124,7 +2395,7 @@
       </c>
       <c r="D55" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -2133,6 +2404,11 @@
       <c r="F55" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G55" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2142,9 +2418,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>J6 Plus / j4 core</t>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>J6</t>
         </is>
       </c>
       <c r="C56" s="7" t="inlineStr">
@@ -2154,7 +2430,7 @@
       </c>
       <c r="D56" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E56" t="n">
@@ -2162,7 +2438,12 @@
       </c>
       <c r="F56" s="7" t="inlineStr">
         <is>
-          <t>J6 +/H2</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G56" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2172,14 +2453,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B57" s="2" t="inlineStr">
-        <is>
-          <t>J7 Prime</t>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>J6 Plus / j4 core</t>
         </is>
       </c>
       <c r="C57" s="7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D57" s="7" t="inlineStr">
@@ -2188,11 +2469,16 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" s="7" t="inlineStr">
         <is>
-          <t>J7 Prime</t>
+          <t>J6 +</t>
+        </is>
+      </c>
+      <c r="G57" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2202,14 +2488,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B58" s="3" t="inlineStr">
+      <c r="B58" s="2" t="inlineStr">
         <is>
           <t>J7 Prime</t>
         </is>
       </c>
       <c r="C58" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="D58" s="7" t="inlineStr">
@@ -2223,6 +2509,11 @@
       <c r="F58" s="7" t="inlineStr">
         <is>
           <t>J7 Prime</t>
+        </is>
+      </c>
+      <c r="G58" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2232,14 +2523,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B59" s="2" t="inlineStr">
-        <is>
-          <t>J7 Prime 2</t>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>J7 Prime</t>
         </is>
       </c>
       <c r="C59" s="7" t="inlineStr">
         <is>
-          <t>Marrom</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D59" s="7" t="inlineStr">
@@ -2248,11 +2539,16 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" s="7" t="inlineStr">
         <is>
           <t>J7 Prime</t>
+        </is>
+      </c>
+      <c r="G59" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2262,14 +2558,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B60" s="3" t="inlineStr">
-        <is>
-          <t>J7 Pro</t>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>J7 Prime 2</t>
         </is>
       </c>
       <c r="C60" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Marrom</t>
         </is>
       </c>
       <c r="D60" s="7" t="inlineStr">
@@ -2278,11 +2574,16 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F60" s="7" t="inlineStr">
         <is>
-          <t>Samsung Orig. Importada</t>
+          <t>J7 Prime</t>
+        </is>
+      </c>
+      <c r="G60" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2292,14 +2593,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B61" s="2" t="inlineStr">
+      <c r="B61" s="3" t="inlineStr">
         <is>
           <t>J7 Pro</t>
         </is>
       </c>
       <c r="C61" s="7" t="inlineStr">
         <is>
-          <t>Dourada</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D61" s="7" t="inlineStr">
@@ -2313,6 +2614,11 @@
       <c r="F61" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G61" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2322,27 +2628,32 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B62" s="3" t="inlineStr">
-        <is>
-          <t>J8</t>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>J7 Pro</t>
         </is>
       </c>
       <c r="C62" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Dourada</t>
         </is>
       </c>
       <c r="D62" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G62" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2352,14 +2663,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B63" s="2" t="inlineStr">
-        <is>
-          <t>J7</t>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>J8</t>
         </is>
       </c>
       <c r="C63" s="7" t="inlineStr">
         <is>
-          <t>Dourada</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D63" s="7" t="inlineStr">
@@ -2368,11 +2679,16 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G63" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2382,27 +2698,32 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr">
-        <is>
-          <t>A01</t>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>J7</t>
         </is>
       </c>
       <c r="C64" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Dourada</t>
         </is>
       </c>
       <c r="D64" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" s="7" t="inlineStr">
         <is>
-          <t>A01 A10 A10s</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G64" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2412,9 +2733,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B65" s="2" t="inlineStr">
-        <is>
-          <t>A01 Core</t>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>A01</t>
         </is>
       </c>
       <c r="C65" s="7" t="inlineStr">
@@ -2428,11 +2749,16 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F65" s="7" t="inlineStr">
         <is>
           <t>A01 A10 A10s</t>
+        </is>
+      </c>
+      <c r="G65" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2442,9 +2768,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B66" s="4" t="inlineStr">
-        <is>
-          <t>A02</t>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>A01 Core</t>
         </is>
       </c>
       <c r="C66" s="7" t="inlineStr">
@@ -2462,7 +2788,12 @@
       </c>
       <c r="F66" s="7" t="inlineStr">
         <is>
-          <t>Samsung Orig. Importada</t>
+          <t>A01 A10 A10s</t>
+        </is>
+      </c>
+      <c r="G66" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2472,9 +2803,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr">
-        <is>
-          <t>A02s</t>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>A02</t>
         </is>
       </c>
       <c r="C67" s="7" t="inlineStr">
@@ -2492,7 +2823,12 @@
       </c>
       <c r="F67" s="7" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G67" s="7" t="inlineStr">
+        <is>
+          <t>E76</t>
         </is>
       </c>
     </row>
@@ -2502,9 +2838,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B68" s="4" t="inlineStr">
-        <is>
-          <t>A03</t>
+      <c r="B68" s="6" t="inlineStr">
+        <is>
+          <t>A022F</t>
         </is>
       </c>
       <c r="C68" s="7" t="inlineStr">
@@ -2514,7 +2850,7 @@
       </c>
       <c r="D68" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E68" t="n">
@@ -2522,7 +2858,12 @@
       </c>
       <c r="F68" s="7" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G68" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2532,9 +2873,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B69" s="2" t="inlineStr">
-        <is>
-          <t>A03s</t>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>A02s</t>
         </is>
       </c>
       <c r="C69" s="7" t="inlineStr">
@@ -2552,7 +2893,12 @@
       </c>
       <c r="F69" s="7" t="inlineStr">
         <is>
-          <t>Samsung/H2</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G69" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2562,9 +2908,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr">
-        <is>
-          <t>A10</t>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>A03</t>
         </is>
       </c>
       <c r="C70" s="7" t="inlineStr">
@@ -2582,7 +2928,12 @@
       </c>
       <c r="F70" s="7" t="inlineStr">
         <is>
-          <t>A01 A10 A10s</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G70" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2592,9 +2943,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr">
-        <is>
-          <t>A10s</t>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>A03s</t>
         </is>
       </c>
       <c r="C71" s="7" t="inlineStr">
@@ -2608,11 +2959,16 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="7" t="inlineStr">
         <is>
-          <t>A01 A10 A10s</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G71" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2622,9 +2978,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B72" s="4" t="inlineStr">
-        <is>
-          <t>A12</t>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>A10</t>
         </is>
       </c>
       <c r="C72" s="7" t="inlineStr">
@@ -2642,7 +2998,12 @@
       </c>
       <c r="F72" s="7" t="inlineStr">
         <is>
-          <t>Samsung Orig. Importada</t>
+          <t>A01 A10 A10s</t>
+        </is>
+      </c>
+      <c r="G72" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2654,7 +3015,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>A11</t>
+          <t>A10s</t>
         </is>
       </c>
       <c r="C73" s="7" t="inlineStr">
@@ -2668,11 +3029,16 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" s="7" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>A01 A10 A10s</t>
+        </is>
+      </c>
+      <c r="G73" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2682,9 +3048,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B74" s="2" t="inlineStr">
-        <is>
-          <t>A12/A02</t>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>A12</t>
         </is>
       </c>
       <c r="C74" s="7" t="inlineStr">
@@ -2694,15 +3060,20 @@
       </c>
       <c r="D74" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F74" s="7" t="inlineStr">
         <is>
           <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G74" s="7" t="inlineStr">
+        <is>
+          <t>E76</t>
         </is>
       </c>
     </row>
@@ -2714,7 +3085,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>A20s</t>
+          <t>A11</t>
         </is>
       </c>
       <c r="C75" s="7" t="inlineStr">
@@ -2728,11 +3099,16 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="7" t="inlineStr">
         <is>
-          <t>A20s/H2</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G75" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2744,7 +3120,7 @@
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>A21s</t>
+          <t>A12/A02</t>
         </is>
       </c>
       <c r="C76" s="7" t="inlineStr">
@@ -2754,15 +3130,20 @@
       </c>
       <c r="D76" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F76" s="7" t="inlineStr">
         <is>
-          <t>Samsung/H2</t>
+          <t>Samsung Orig. Importada</t>
+        </is>
+      </c>
+      <c r="G76" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2774,7 +3155,7 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>A30s original china</t>
+          <t>A20s</t>
         </is>
       </c>
       <c r="C77" s="7" t="inlineStr">
@@ -2784,15 +3165,20 @@
       </c>
       <c r="D77" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="7" t="inlineStr">
         <is>
-          <t>Samsung</t>
+          <t>A20s</t>
+        </is>
+      </c>
+      <c r="G77" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2804,25 +3190,30 @@
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>A30 original china</t>
+          <t>A21s</t>
         </is>
       </c>
       <c r="C78" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Preta </t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D78" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="7" t="inlineStr">
         <is>
           <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G78" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2832,9 +3223,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B79" s="4" t="inlineStr">
-        <is>
-          <t>A32 4G</t>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>A30s original china</t>
         </is>
       </c>
       <c r="C79" s="7" t="inlineStr">
@@ -2853,6 +3244,11 @@
       <c r="F79" s="7" t="inlineStr">
         <is>
           <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G79" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2862,14 +3258,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr">
-        <is>
-          <t>A50 original nacional aro</t>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>A30 original china</t>
         </is>
       </c>
       <c r="C80" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t xml:space="preserve">Preta </t>
         </is>
       </c>
       <c r="D80" s="7" t="inlineStr">
@@ -2885,6 +3281,11 @@
           <t>Samsung</t>
         </is>
       </c>
+      <c r="G80" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="7" t="inlineStr">
@@ -2892,9 +3293,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B81" s="6" t="inlineStr">
-        <is>
-          <t>M12</t>
+      <c r="B81" s="4" t="inlineStr">
+        <is>
+          <t>A32 4G</t>
         </is>
       </c>
       <c r="C81" s="7" t="inlineStr">
@@ -2913,6 +3314,11 @@
       <c r="F81" s="7" t="inlineStr">
         <is>
           <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G81" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2922,9 +3328,9 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
-          <t>M20</t>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>A50 original nacional aro</t>
         </is>
       </c>
       <c r="C82" s="7" t="inlineStr">
@@ -2938,11 +3344,16 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F82" s="7" t="inlineStr">
         <is>
           <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G82" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2952,14 +3363,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B83" s="2" t="inlineStr">
-        <is>
-          <t>Touch G530</t>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>M12</t>
         </is>
       </c>
       <c r="C83" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D83" s="7" t="inlineStr">
@@ -2968,11 +3379,16 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83" s="7" t="inlineStr">
         <is>
-          <t>Touch Display G530</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G83" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -2982,14 +3398,14 @@
           <t>Samsung</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr">
-        <is>
-          <t>Touch G530</t>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>M20</t>
         </is>
       </c>
       <c r="C84" s="7" t="inlineStr">
         <is>
-          <t>Dourado</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D84" s="7" t="inlineStr">
@@ -2998,11 +3414,16 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F84" s="7" t="inlineStr">
         <is>
-          <t>Touch Display G530</t>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="G84" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3019,7 +3440,7 @@
       </c>
       <c r="C85" s="7" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D85" s="7" t="inlineStr">
@@ -3028,11 +3449,16 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F85" s="7" t="inlineStr">
         <is>
           <t>Touch Display G530</t>
+        </is>
+      </c>
+      <c r="G85" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3044,12 +3470,12 @@
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Touch G532</t>
+          <t>Touch G530</t>
         </is>
       </c>
       <c r="C86" s="7" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Dourado</t>
         </is>
       </c>
       <c r="D86" s="7" t="inlineStr">
@@ -3058,11 +3484,16 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F86" s="7" t="inlineStr">
         <is>
           <t>Touch Display G530</t>
+        </is>
+      </c>
+      <c r="G86" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3074,12 +3505,12 @@
       </c>
       <c r="B87" s="2" t="inlineStr">
         <is>
-          <t>Touch G532</t>
+          <t>Touch G530</t>
         </is>
       </c>
       <c r="C87" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="D87" s="7" t="inlineStr">
@@ -3088,11 +3519,16 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="7" t="inlineStr">
         <is>
           <t>Touch Display G530</t>
+        </is>
+      </c>
+      <c r="G87" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3545,7 @@
       </c>
       <c r="C88" s="7" t="inlineStr">
         <is>
-          <t>Dourada</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="D88" s="7" t="inlineStr">
@@ -3125,6 +3561,11 @@
           <t>Touch Display G530</t>
         </is>
       </c>
+      <c r="G88" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="7" t="inlineStr">
@@ -3134,12 +3575,12 @@
       </c>
       <c r="B89" s="2" t="inlineStr">
         <is>
-          <t>Display G530</t>
+          <t>Touch G532</t>
         </is>
       </c>
       <c r="C89" s="7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D89" s="7" t="inlineStr">
@@ -3155,56 +3596,66 @@
           <t>Touch Display G530</t>
         </is>
       </c>
+      <c r="G89" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="7" t="inlineStr">
         <is>
-          <t>LG</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>K10</t>
+          <t>Touch G532</t>
         </is>
       </c>
       <c r="C90" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Dourada</t>
         </is>
       </c>
       <c r="D90" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F90" s="7" t="inlineStr">
         <is>
-          <t>LG 2</t>
+          <t>Touch Display G530</t>
+        </is>
+      </c>
+      <c r="G90" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="7" t="inlineStr">
         <is>
-          <t>LG</t>
+          <t>Samsung</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
         <is>
-          <t>K10 2017</t>
+          <t>Display G530</t>
         </is>
       </c>
       <c r="C91" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D91" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -3212,7 +3663,12 @@
       </c>
       <c r="F91" s="7" t="inlineStr">
         <is>
-          <t>LG 2</t>
+          <t>Touch Display G530</t>
+        </is>
+      </c>
+      <c r="G91" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3224,7 +3680,7 @@
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>K4 2017 C/Aro</t>
+          <t>K10</t>
         </is>
       </c>
       <c r="C92" s="7" t="inlineStr">
@@ -3238,11 +3694,16 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F92" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G92" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3715,7 @@
       </c>
       <c r="B93" s="2" t="inlineStr">
         <is>
-          <t>K40/K40s</t>
+          <t>K10 2017</t>
         </is>
       </c>
       <c r="C93" s="7" t="inlineStr">
@@ -3264,15 +3725,20 @@
       </c>
       <c r="D93" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G93" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3282,19 +3748,19 @@
           <t>LG</t>
         </is>
       </c>
-      <c r="B94" s="4" t="inlineStr">
-        <is>
-          <t>K12 Max</t>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>K10 Power</t>
         </is>
       </c>
       <c r="C94" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Dourada</t>
         </is>
       </c>
       <c r="D94" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -3303,6 +3769,11 @@
       <c r="F94" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G94" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3312,9 +3783,9 @@
           <t>LG</t>
         </is>
       </c>
-      <c r="B95" s="6" t="inlineStr">
-        <is>
-          <t>K12 Plus</t>
+      <c r="B95" s="2" t="inlineStr">
+        <is>
+          <t>K40/K40s</t>
         </is>
       </c>
       <c r="C95" s="7" t="inlineStr">
@@ -3335,6 +3806,11 @@
           <t>LG 2</t>
         </is>
       </c>
+      <c r="G95" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="7" t="inlineStr">
@@ -3342,9 +3818,9 @@
           <t>LG</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>K9 C/Aro</t>
+      <c r="B96" s="4" t="inlineStr">
+        <is>
+          <t>K12 Max</t>
         </is>
       </c>
       <c r="C96" s="7" t="inlineStr">
@@ -3354,7 +3830,7 @@
       </c>
       <c r="D96" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -3363,6 +3839,11 @@
       <c r="F96" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G96" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3372,9 +3853,9 @@
           <t>LG</t>
         </is>
       </c>
-      <c r="B97" s="2" t="inlineStr">
-        <is>
-          <t>K11 Plus C/Aro</t>
+      <c r="B97" s="6" t="inlineStr">
+        <is>
+          <t>K12 Plus</t>
         </is>
       </c>
       <c r="C97" s="7" t="inlineStr">
@@ -3395,6 +3876,11 @@
           <t>LG 2</t>
         </is>
       </c>
+      <c r="G97" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="7" t="inlineStr">
@@ -3404,7 +3890,7 @@
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>K11 C/Aro</t>
+          <t>K9 C/Aro</t>
         </is>
       </c>
       <c r="C98" s="7" t="inlineStr">
@@ -3414,7 +3900,7 @@
       </c>
       <c r="D98" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -3423,6 +3909,11 @@
       <c r="F98" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G98" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3434,7 +3925,7 @@
       </c>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>K22/22+</t>
+          <t>K11 Plus C/Aro</t>
         </is>
       </c>
       <c r="C99" s="7" t="inlineStr">
@@ -3448,11 +3939,16 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F99" s="7" t="inlineStr">
         <is>
-          <t>LG 2/H2</t>
+          <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G99" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3464,7 +3960,7 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>K8 Plus</t>
+          <t>K11 C/Aro</t>
         </is>
       </c>
       <c r="C100" s="7" t="inlineStr">
@@ -3474,15 +3970,20 @@
       </c>
       <c r="D100" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="7" t="inlineStr">
         <is>
           <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G100" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3494,7 +3995,7 @@
       </c>
       <c r="B101" s="2" t="inlineStr">
         <is>
-          <t>X Power C/Aro</t>
+          <t>K22/22+</t>
         </is>
       </c>
       <c r="C101" s="7" t="inlineStr">
@@ -3504,7 +4005,7 @@
       </c>
       <c r="D101" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -3512,7 +4013,12 @@
       </c>
       <c r="F101" s="7" t="inlineStr">
         <is>
-          <t>LG 2</t>
+          <t>LG 2/H2</t>
+        </is>
+      </c>
+      <c r="G101" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3524,25 +4030,30 @@
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Touch K4</t>
+          <t>K8 Plus</t>
         </is>
       </c>
       <c r="C102" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D102" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">LG </t>
+          <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G102" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3554,12 +4065,12 @@
       </c>
       <c r="B103" s="2" t="inlineStr">
         <is>
-          <t>Display K4</t>
+          <t>X Power C/Aro</t>
         </is>
       </c>
       <c r="C103" s="7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D103" s="7" t="inlineStr">
@@ -3568,28 +4079,33 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">LG  </t>
+          <t>LG 2</t>
+        </is>
+      </c>
+      <c r="G103" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="7" t="inlineStr">
         <is>
-          <t>Iphone</t>
+          <t>LG</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>4G</t>
+          <t>Touch K4</t>
         </is>
       </c>
       <c r="C104" s="7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D104" s="7" t="inlineStr">
@@ -3602,37 +4118,47 @@
       </c>
       <c r="F104" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 2</t>
+          <t xml:space="preserve">LG </t>
+        </is>
+      </c>
+      <c r="G104" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="7" t="inlineStr">
         <is>
-          <t>Iphone</t>
+          <t>LG</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
         <is>
-          <t>5G</t>
+          <t>Display K4</t>
         </is>
       </c>
       <c r="C105" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D105" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E105" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F105" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 2</t>
+          <t xml:space="preserve">LG  </t>
+        </is>
+      </c>
+      <c r="G105" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3644,7 +4170,7 @@
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>5G</t>
+          <t>4G</t>
         </is>
       </c>
       <c r="C106" s="7" t="inlineStr">
@@ -3654,7 +4180,7 @@
       </c>
       <c r="D106" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -3663,6 +4189,11 @@
       <c r="F106" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G106" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3674,7 +4205,7 @@
       </c>
       <c r="B107" s="2" t="inlineStr">
         <is>
-          <t>5S</t>
+          <t>5G</t>
         </is>
       </c>
       <c r="C107" s="7" t="inlineStr">
@@ -3688,11 +4219,16 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F107" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G107" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3704,7 +4240,7 @@
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>5S</t>
+          <t>5G</t>
         </is>
       </c>
       <c r="C108" s="7" t="inlineStr">
@@ -3718,11 +4254,16 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G108" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3734,12 +4275,12 @@
       </c>
       <c r="B109" s="2" t="inlineStr">
         <is>
-          <t>5SE</t>
+          <t>5S</t>
         </is>
       </c>
       <c r="C109" s="7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D109" s="7" t="inlineStr">
@@ -3755,6 +4296,11 @@
           <t>Iphone Caixa 2</t>
         </is>
       </c>
+      <c r="G109" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="7" t="inlineStr">
@@ -3764,25 +4310,30 @@
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>6G</t>
+          <t>5S</t>
         </is>
       </c>
       <c r="C110" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="D110" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F110" s="7" t="inlineStr">
         <is>
-          <t>Frontal Iphone</t>
+          <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G110" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3794,7 +4345,7 @@
       </c>
       <c r="B111" s="2" t="inlineStr">
         <is>
-          <t>6G</t>
+          <t>5SE</t>
         </is>
       </c>
       <c r="C111" s="7" t="inlineStr">
@@ -3804,15 +4355,20 @@
       </c>
       <c r="D111" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F111" s="7" t="inlineStr">
         <is>
-          <t>Frontal Iphone</t>
+          <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G111" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3824,7 +4380,7 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>6S</t>
+          <t>6G</t>
         </is>
       </c>
       <c r="C112" s="7" t="inlineStr">
@@ -3838,11 +4394,16 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F112" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G112" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3854,7 +4415,7 @@
       </c>
       <c r="B113" s="2" t="inlineStr">
         <is>
-          <t>6S</t>
+          <t>6G</t>
         </is>
       </c>
       <c r="C113" s="7" t="inlineStr">
@@ -3873,6 +4434,11 @@
       <c r="F113" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G113" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3884,7 +4450,7 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>6 Plus</t>
+          <t>6S</t>
         </is>
       </c>
       <c r="C114" s="7" t="inlineStr">
@@ -3898,11 +4464,16 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F114" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G114" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3914,7 +4485,7 @@
       </c>
       <c r="B115" s="2" t="inlineStr">
         <is>
-          <t>6 Plus</t>
+          <t>6S</t>
         </is>
       </c>
       <c r="C115" s="7" t="inlineStr">
@@ -3928,11 +4499,16 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F115" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G115" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3944,7 +4520,7 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>6s Plus</t>
+          <t>6 Plus</t>
         </is>
       </c>
       <c r="C116" s="7" t="inlineStr">
@@ -3958,11 +4534,16 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F116" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G116" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -3974,7 +4555,7 @@
       </c>
       <c r="B117" s="2" t="inlineStr">
         <is>
-          <t>6s Plus</t>
+          <t>6 Plus</t>
         </is>
       </c>
       <c r="C117" s="7" t="inlineStr">
@@ -3988,11 +4569,16 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F117" s="7" t="inlineStr">
         <is>
           <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G117" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4004,12 +4590,12 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>7G</t>
+          <t>6s Plus</t>
         </is>
       </c>
       <c r="C118" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D118" s="7" t="inlineStr">
@@ -4022,7 +4608,12 @@
       </c>
       <c r="F118" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 4</t>
+          <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G118" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4034,7 +4625,7 @@
       </c>
       <c r="B119" s="2" t="inlineStr">
         <is>
-          <t>7G</t>
+          <t>6s Plus</t>
         </is>
       </c>
       <c r="C119" s="7" t="inlineStr">
@@ -4048,11 +4639,16 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F119" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 4</t>
+          <t>Frontal Iphone</t>
+        </is>
+      </c>
+      <c r="G119" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4064,12 +4660,12 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>7 Plus</t>
+          <t>7G</t>
         </is>
       </c>
       <c r="C120" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="D120" s="7" t="inlineStr">
@@ -4078,11 +4674,16 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F120" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G120" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4094,7 +4695,7 @@
       </c>
       <c r="B121" s="2" t="inlineStr">
         <is>
-          <t>7 Plus</t>
+          <t>7G</t>
         </is>
       </c>
       <c r="C121" s="7" t="inlineStr">
@@ -4108,11 +4709,16 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F121" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G121" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4124,7 +4730,7 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>8G</t>
+          <t>7 Plus</t>
         </is>
       </c>
       <c r="C122" s="7" t="inlineStr">
@@ -4138,11 +4744,16 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F122" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G122" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4154,7 +4765,7 @@
       </c>
       <c r="B123" s="2" t="inlineStr">
         <is>
-          <t>8G</t>
+          <t>7 Plus</t>
         </is>
       </c>
       <c r="C123" s="7" t="inlineStr">
@@ -4173,6 +4784,11 @@
       <c r="F123" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G123" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4184,7 +4800,7 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>8 plus</t>
+          <t>8G</t>
         </is>
       </c>
       <c r="C124" s="7" t="inlineStr">
@@ -4203,6 +4819,11 @@
       <c r="F124" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G124" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4214,7 +4835,7 @@
       </c>
       <c r="B125" s="2" t="inlineStr">
         <is>
-          <t>8 plus</t>
+          <t>8G</t>
         </is>
       </c>
       <c r="C125" s="7" t="inlineStr">
@@ -4228,11 +4849,16 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F125" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G125" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4242,9 +4868,9 @@
           <t>Iphone</t>
         </is>
       </c>
-      <c r="B126" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
+      <c r="B126" s="3" t="inlineStr">
+        <is>
+          <t>8 plus</t>
         </is>
       </c>
       <c r="C126" s="7" t="inlineStr">
@@ -4254,7 +4880,7 @@
       </c>
       <c r="D126" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E126" t="n">
@@ -4262,7 +4888,12 @@
       </c>
       <c r="F126" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 2</t>
+          <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G126" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4272,27 +4903,32 @@
           <t>Iphone</t>
         </is>
       </c>
-      <c r="B127" s="3" t="inlineStr">
-        <is>
-          <t>Iphone 11</t>
+      <c r="B127" s="2" t="inlineStr">
+        <is>
+          <t>8 plus</t>
         </is>
       </c>
       <c r="C127" s="7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="D127" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F127" s="7" t="inlineStr">
         <is>
-          <t>Iphone Caixa 2</t>
+          <t>Iphone Caixa 4</t>
+        </is>
+      </c>
+      <c r="G127" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4302,9 +4938,9 @@
           <t>Iphone</t>
         </is>
       </c>
-      <c r="B128" s="6" t="inlineStr">
-        <is>
-          <t>11 Pro Max</t>
+      <c r="B128" s="4" t="inlineStr">
+        <is>
+          <t>X</t>
         </is>
       </c>
       <c r="C128" s="7" t="inlineStr">
@@ -4314,27 +4950,32 @@
       </c>
       <c r="D128" s="7" t="inlineStr">
         <is>
-          <t>Médio Baixo</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F128" s="7" t="inlineStr">
         <is>
           <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G128" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="7" t="inlineStr">
         <is>
-          <t>Asus</t>
-        </is>
-      </c>
-      <c r="B129" s="2" t="inlineStr">
-        <is>
-          <t>Go Mini452</t>
+          <t>Iphone</t>
+        </is>
+      </c>
+      <c r="B129" s="3" t="inlineStr">
+        <is>
+          <t>Iphone 11</t>
         </is>
       </c>
       <c r="C129" s="7" t="inlineStr">
@@ -4344,27 +4985,32 @@
       </c>
       <c r="D129" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F129" s="7" t="inlineStr">
         <is>
-          <t>Vários Modelos Fron.</t>
+          <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G129" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="inlineStr">
         <is>
-          <t>Asus</t>
-        </is>
-      </c>
-      <c r="B130" s="3" t="inlineStr">
-        <is>
-          <t>ZB551KL</t>
+          <t>Iphone</t>
+        </is>
+      </c>
+      <c r="B130" s="6" t="inlineStr">
+        <is>
+          <t>11 Pro Max</t>
         </is>
       </c>
       <c r="C130" s="7" t="inlineStr">
@@ -4374,7 +5020,7 @@
       </c>
       <c r="D130" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Médio Baixo</t>
         </is>
       </c>
       <c r="E130" t="n">
@@ -4382,7 +5028,12 @@
       </c>
       <c r="F130" s="7" t="inlineStr">
         <is>
-          <t>Vários Modelos Fron.</t>
+          <t>Iphone Caixa 2</t>
+        </is>
+      </c>
+      <c r="G130" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4394,12 +5045,12 @@
       </c>
       <c r="B131" s="2" t="inlineStr">
         <is>
-          <t>ZE552KL</t>
+          <t>Go Mini452</t>
         </is>
       </c>
       <c r="C131" s="7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D131" s="7" t="inlineStr">
@@ -4413,18 +5064,23 @@
       <c r="F131" s="7" t="inlineStr">
         <is>
           <t>Vários Modelos Fron.</t>
+        </is>
+      </c>
+      <c r="G131" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="7" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>Asus</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>ZB551KL</t>
         </is>
       </c>
       <c r="C132" s="7" t="inlineStr">
@@ -4434,7 +5090,7 @@
       </c>
       <c r="D132" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E132" t="n">
@@ -4442,67 +5098,82 @@
       </c>
       <c r="F132" s="7" t="inlineStr">
         <is>
-          <t>Nokia 2.4</t>
+          <t>Vários Modelos Fron.</t>
+        </is>
+      </c>
+      <c r="G132" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="7" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Asus</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
         <is>
-          <t>Redmi Note 7</t>
+          <t>ZE552KL</t>
         </is>
       </c>
       <c r="C133" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="D133" s="7" t="inlineStr">
         <is>
-          <t>Alto</t>
+          <t>Exceção</t>
         </is>
       </c>
       <c r="E133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F133" s="7" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Vários Modelos Fron.</t>
+        </is>
+      </c>
+      <c r="G133" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="7" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Nokia</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>Redmi Note 7 Pro</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="C134" s="7" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="D134" s="7" t="inlineStr">
         <is>
-          <t>Médio</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" s="7" t="inlineStr">
         <is>
-          <t>Xiaomi</t>
+          <t>Nokia 2.4</t>
+        </is>
+      </c>
+      <c r="G134" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4514,7 +5185,7 @@
       </c>
       <c r="B135" s="2" t="inlineStr">
         <is>
-          <t>Redmi Note 8</t>
+          <t>Redmi Note 7</t>
         </is>
       </c>
       <c r="C135" s="7" t="inlineStr">
@@ -4533,6 +5204,11 @@
       <c r="F135" s="7" t="inlineStr">
         <is>
           <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="G135" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4542,9 +5218,9 @@
           <t>Xiaomi</t>
         </is>
       </c>
-      <c r="B136" s="3" t="inlineStr">
-        <is>
-          <t>Redmi note 9s</t>
+      <c r="B136" s="2" t="inlineStr">
+        <is>
+          <t>Redmi Note 8</t>
         </is>
       </c>
       <c r="C136" s="7" t="inlineStr">
@@ -4554,15 +5230,20 @@
       </c>
       <c r="D136" s="7" t="inlineStr">
         <is>
-          <t>Baixo</t>
+          <t>Alto</t>
         </is>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" s="7" t="inlineStr">
         <is>
           <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="G136" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
@@ -4572,9 +5253,9 @@
           <t>Xiaomi</t>
         </is>
       </c>
-      <c r="B137" s="2" t="inlineStr">
-        <is>
-          <t>Xiaomi Mi Play</t>
+      <c r="B137" s="3" t="inlineStr">
+        <is>
+          <t>Redmi note 9s</t>
         </is>
       </c>
       <c r="C137" s="7" t="inlineStr">
@@ -4584,27 +5265,32 @@
       </c>
       <c r="D137" s="7" t="inlineStr">
         <is>
-          <t>Exceção</t>
+          <t>Baixo</t>
         </is>
       </c>
       <c r="E137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F137" s="7" t="inlineStr">
         <is>
           <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="G137" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="inlineStr">
         <is>
-          <t>Sony</t>
-        </is>
-      </c>
-      <c r="B138" s="3" t="inlineStr">
-        <is>
-          <t>Z3 Mini</t>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="B138" s="2" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi Play</t>
         </is>
       </c>
       <c r="C138" s="7" t="inlineStr">
@@ -4622,24 +5308,64 @@
       </c>
       <c r="F138" s="7" t="inlineStr">
         <is>
-          <t>Vários Modelos Fron.</t>
+          <t>Xiaomi</t>
+        </is>
+      </c>
+      <c r="G138" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="inlineStr">
         <is>
+          <t>Sony</t>
+        </is>
+      </c>
+      <c r="B139" s="3" t="inlineStr">
+        <is>
+          <t>Z3 Mini</t>
+        </is>
+      </c>
+      <c r="C139" s="7" t="inlineStr">
+        <is>
+          <t>Preto</t>
+        </is>
+      </c>
+      <c r="D139" s="7" t="inlineStr">
+        <is>
+          <t>Exceção</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>1</v>
+      </c>
+      <c r="F139" s="7" t="inlineStr">
+        <is>
+          <t>Vários Modelos Fron.</t>
+        </is>
+      </c>
+      <c r="G139" s="7" t="inlineStr">
+        <is>
+          <t>Vazio</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="7" t="inlineStr">
+        <is>
           <t>Fim</t>
         </is>
       </c>
-      <c r="D139" s="7" t="n"/>
-      <c r="E139" s="5">
-        <f>SUM(E2:E138)</f>
+      <c r="D140" s="7" t="n"/>
+      <c r="E140" s="5">
+        <f>SUM(E2:E139)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:C138 E2:E138">
+  <conditionalFormatting sqref="A2:C139 E2:E139">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4651,8 +5377,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E138">
-    <cfRule type="colorScale" priority="192">
+  <conditionalFormatting sqref="E2:E139">
+    <cfRule type="colorScale" priority="251">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4662,7 +5388,7 @@
         <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="193">
+    <cfRule type="colorScale" priority="252">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4672,7 +5398,7 @@
         <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="194">
+    <cfRule type="colorScale" priority="253">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>